<commit_message>
csv en excel kan gelezen worden met gekozen kolom index
</commit_message>
<xml_diff>
--- a/src/data/xlsxDouble.xlsx
+++ b/src/data/xlsxDouble.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Sem1_2021_2022\SEM2\SDP2\eclipse\2022-java-gr10\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13121605-182C-46A3-A485-C0B5411EAE67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883FB9E8-910E-4338-B1ED-0FEECC35F950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3645" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{C51259E9-AF76-4A08-8FBA-22B96DCECE69}"/>
+    <workbookView xWindow="4695" yWindow="3585" windowWidth="21600" windowHeight="11115" xr2:uid="{C51259E9-AF76-4A08-8FBA-22B96DCECE69}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,21 +35,51 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>5.6</t>
   </si>
   <si>
-    <t>3.9</t>
-  </si>
-  <si>
-    <t>8.5</t>
-  </si>
-  <si>
-    <t>6.4</t>
-  </si>
-  <si>
-    <t>xlsx</t>
+    <t>co2 mercedes</t>
+  </si>
+  <si>
+    <t>co2 audi</t>
+  </si>
+  <si>
+    <t>co2 bmw</t>
+  </si>
+  <si>
+    <t>7.9</t>
+  </si>
+  <si>
+    <t>9.5</t>
+  </si>
+  <si>
+    <t>3.8</t>
+  </si>
+  <si>
+    <t>8.4</t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>9.4</t>
+  </si>
+  <si>
+    <t>1.6</t>
+  </si>
+  <si>
+    <t>10.4</t>
+  </si>
+  <si>
+    <t>15.6</t>
+  </si>
+  <si>
+    <t>4.8</t>
+  </si>
+  <si>
+    <t>16.4</t>
   </si>
 </sst>
 </file>
@@ -401,35 +431,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0940D15F-1E80-45BB-986C-BB63032A7DA2}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>